<commit_message>
MDS database is updated but ProductSILog table is still deleted from database, it will be added lator on....
</commit_message>
<xml_diff>
--- a/Data Dictionary Version 0.xlsx
+++ b/Data Dictionary Version 0.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="861">
   <si>
     <t xml:space="preserve">T2</t>
   </si>
@@ -2008,6 +2008,15 @@
   </si>
   <si>
     <t xml:space="preserve">store 1 for quantity in kg else store 0 for per litre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnimalName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Char(20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store  animal name of which customer is bought milk</t>
   </si>
   <si>
     <t xml:space="preserve">T52</t>
@@ -2965,20 +2974,20 @@
   </sheetPr>
   <dimension ref="A3:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A529" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A550" activeCellId="0" sqref="A550"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C529" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C552" activeCellId="0" sqref="C552"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -11851,12 +11860,35 @@
         <v>661</v>
       </c>
     </row>
+    <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A551" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B551" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="C551" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="D551" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E551" s="7"/>
+      <c r="F551" s="7"/>
+      <c r="G551" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="H551" s="7"/>
+      <c r="I551" s="7" t="s">
+        <v>664</v>
+      </c>
+    </row>
     <row r="553" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="1" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11905,12 +11937,12 @@
         <v>90</v>
       </c>
       <c r="F556" s="8" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="G556" s="8"/>
       <c r="H556" s="8"/>
       <c r="I556" s="8" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11937,7 +11969,7 @@
         <v>42</v>
       </c>
       <c r="I557" s="7" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11962,7 +11994,7 @@
         <v>414</v>
       </c>
       <c r="I558" s="8" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11985,7 +12017,7 @@
       </c>
       <c r="H559" s="7"/>
       <c r="I559" s="7" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12010,7 +12042,7 @@
       <c r="G560" s="8"/>
       <c r="H560" s="8"/>
       <c r="I560" s="8" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12018,7 +12050,7 @@
         <v>6</v>
       </c>
       <c r="B561" s="7" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="C561" s="7" t="s">
         <v>109</v>
@@ -12031,7 +12063,7 @@
       <c r="G561" s="7"/>
       <c r="H561" s="7"/>
       <c r="I561" s="7" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12039,7 +12071,7 @@
         <v>7</v>
       </c>
       <c r="B562" s="8" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="C562" s="8" t="s">
         <v>366</v>
@@ -12052,7 +12084,7 @@
       <c r="G562" s="8"/>
       <c r="H562" s="8"/>
       <c r="I562" s="8" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12063,7 +12095,7 @@
         <v>614</v>
       </c>
       <c r="C563" s="7" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="D563" s="7" t="s">
         <v>13</v>
@@ -12096,7 +12128,7 @@
       </c>
       <c r="H564" s="8"/>
       <c r="I564" s="8" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12140,7 +12172,7 @@
       <c r="G566" s="8"/>
       <c r="H566" s="8"/>
       <c r="I566" s="8" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
     </row>
     <row r="567" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12161,7 +12193,7 @@
       <c r="G567" s="7"/>
       <c r="H567" s="7"/>
       <c r="I567" s="7" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
     </row>
     <row r="568" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12184,7 +12216,7 @@
       </c>
       <c r="H568" s="8"/>
       <c r="I568" s="8" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
     </row>
     <row r="569" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12209,7 +12241,7 @@
       <c r="G569" s="7"/>
       <c r="H569" s="7"/>
       <c r="I569" s="7" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
     <row r="570" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12239,10 +12271,10 @@
     </row>
     <row r="573" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="1" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
     </row>
     <row r="575" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12291,12 +12323,12 @@
         <v>90</v>
       </c>
       <c r="F576" s="8" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="G576" s="8"/>
       <c r="H576" s="8"/>
       <c r="I576" s="8" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="577" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12348,7 +12380,7 @@
         <v>414</v>
       </c>
       <c r="I578" s="8" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
     </row>
     <row r="579" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12356,7 +12388,7 @@
         <v>4</v>
       </c>
       <c r="B579" s="7" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="C579" s="7" t="s">
         <v>417</v>
@@ -12369,7 +12401,7 @@
       <c r="G579" s="7"/>
       <c r="H579" s="7"/>
       <c r="I579" s="7" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
     </row>
     <row r="580" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12377,7 +12409,7 @@
         <v>5</v>
       </c>
       <c r="B580" s="8" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="C580" s="8" t="s">
         <v>417</v>
@@ -12390,7 +12422,7 @@
       <c r="G580" s="8"/>
       <c r="H580" s="8"/>
       <c r="I580" s="8" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12398,7 +12430,7 @@
         <v>6</v>
       </c>
       <c r="B581" s="7" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="C581" s="7" t="s">
         <v>417</v>
@@ -12411,7 +12443,7 @@
       <c r="G581" s="7"/>
       <c r="H581" s="7"/>
       <c r="I581" s="7" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
     </row>
     <row r="582" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12419,7 +12451,7 @@
         <v>7</v>
       </c>
       <c r="B582" s="8" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="C582" s="8" t="s">
         <v>417</v>
@@ -12432,7 +12464,7 @@
       <c r="G582" s="8"/>
       <c r="H582" s="8"/>
       <c r="I582" s="8" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
     <row r="583" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12503,7 +12535,7 @@
       <c r="G585" s="7"/>
       <c r="H585" s="7"/>
       <c r="I585" s="7" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="586" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12524,7 +12556,7 @@
       <c r="G586" s="8"/>
       <c r="H586" s="8"/>
       <c r="I586" s="8" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
     <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12565,10 +12597,10 @@
     </row>
     <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="1" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
     </row>
     <row r="591" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12605,7 +12637,7 @@
         <v>1</v>
       </c>
       <c r="B592" s="10" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="C592" s="8" t="s">
         <v>109</v>
@@ -12622,7 +12654,7 @@
       </c>
       <c r="H592" s="8"/>
       <c r="I592" s="8" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
     </row>
     <row r="593" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12630,7 +12662,7 @@
         <v>2</v>
       </c>
       <c r="B593" s="7" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="C593" s="7" t="s">
         <v>78</v>
@@ -12645,15 +12677,15 @@
       </c>
       <c r="H593" s="7"/>
       <c r="I593" s="7" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
     </row>
     <row r="597" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="1" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
     </row>
     <row r="599" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12690,7 +12722,7 @@
         <v>1</v>
       </c>
       <c r="B600" s="10" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="C600" s="8" t="s">
         <v>109</v>
@@ -12707,7 +12739,7 @@
       </c>
       <c r="H600" s="8"/>
       <c r="I600" s="8" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="601" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12715,7 +12747,7 @@
         <v>2</v>
       </c>
       <c r="B601" s="7" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="C601" s="7" t="s">
         <v>81</v>
@@ -12730,15 +12762,15 @@
       </c>
       <c r="H601" s="7"/>
       <c r="I601" s="7" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
     </row>
     <row r="605" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="1" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="B605" s="1" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="607" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12749,7 +12781,7 @@
         <v>3</v>
       </c>
       <c r="C607" s="2" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="D607" s="2" t="s">
         <v>5</v>
@@ -12775,7 +12807,7 @@
         <v>1</v>
       </c>
       <c r="B608" s="10" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="C608" s="8" t="s">
         <v>109</v>
@@ -12792,7 +12824,7 @@
       </c>
       <c r="H608" s="8"/>
       <c r="I608" s="8" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
     </row>
     <row r="609" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12800,7 +12832,7 @@
         <v>2</v>
       </c>
       <c r="B609" s="7" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="C609" s="7" t="s">
         <v>81</v>
@@ -12815,15 +12847,15 @@
       </c>
       <c r="H609" s="7"/>
       <c r="I609" s="7" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A611" s="1" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12860,10 +12892,10 @@
         <v>1</v>
       </c>
       <c r="B614" s="10" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C614" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D614" s="8" t="s">
         <v>13</v>
@@ -12875,7 +12907,7 @@
       <c r="G614" s="8"/>
       <c r="H614" s="8"/>
       <c r="I614" s="8" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12883,7 +12915,7 @@
         <v>2</v>
       </c>
       <c r="B615" s="7" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="C615" s="7" t="s">
         <v>144</v>
@@ -12896,7 +12928,7 @@
       <c r="G615" s="7"/>
       <c r="H615" s="7"/>
       <c r="I615" s="7" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12904,7 +12936,7 @@
         <v>3</v>
       </c>
       <c r="B616" s="8" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="C616" s="8" t="s">
         <v>78</v>
@@ -12917,7 +12949,7 @@
       <c r="G616" s="8"/>
       <c r="H616" s="8"/>
       <c r="I616" s="8" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12938,7 +12970,7 @@
       <c r="G617" s="7"/>
       <c r="H617" s="7"/>
       <c r="I617" s="7" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
     </row>
     <row r="618" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12959,7 +12991,7 @@
       <c r="G618" s="8"/>
       <c r="H618" s="8"/>
       <c r="I618" s="8" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
     </row>
     <row r="619" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12967,7 +12999,7 @@
         <v>6</v>
       </c>
       <c r="B619" s="7" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="C619" s="7" t="s">
         <v>109</v>
@@ -12979,12 +13011,12 @@
         <v>57</v>
       </c>
       <c r="F619" s="7" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="G619" s="7"/>
       <c r="H619" s="7"/>
       <c r="I619" s="7" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
     </row>
     <row r="620" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12992,7 +13024,7 @@
         <v>7</v>
       </c>
       <c r="B620" s="8" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="C620" s="8" t="s">
         <v>109</v>
@@ -13004,12 +13036,12 @@
         <v>57</v>
       </c>
       <c r="F620" s="8" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="G620" s="8"/>
       <c r="H620" s="8"/>
       <c r="I620" s="8" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
     <row r="621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13017,7 +13049,7 @@
         <v>8</v>
       </c>
       <c r="B621" s="7" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="C621" s="7" t="s">
         <v>109</v>
@@ -13029,12 +13061,12 @@
         <v>57</v>
       </c>
       <c r="F621" s="7" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="G621" s="7"/>
       <c r="H621" s="7"/>
       <c r="I621" s="7" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
     </row>
     <row r="622" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13045,7 +13077,7 @@
         <v>10</v>
       </c>
       <c r="C622" s="8" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="D622" s="8" t="s">
         <v>24</v>
@@ -13055,7 +13087,7 @@
       <c r="G622" s="8"/>
       <c r="H622" s="8"/>
       <c r="I622" s="8" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
     </row>
     <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13072,7 +13104,7 @@
         <v>13</v>
       </c>
       <c r="E623" s="5" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F623" s="5" t="s">
         <v>254</v>
@@ -13096,10 +13128,10 @@
     </row>
     <row r="625" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="1" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="B625" s="1" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
     </row>
     <row r="627" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13136,24 +13168,24 @@
         <v>1</v>
       </c>
       <c r="B628" s="10" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C628" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D628" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E628" s="8" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="F628" s="8" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="G628" s="8"/>
       <c r="H628" s="8"/>
       <c r="I628" s="8" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="629" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13161,7 +13193,7 @@
         <v>2</v>
       </c>
       <c r="B629" s="7" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="C629" s="7" t="s">
         <v>81</v>
@@ -13172,11 +13204,11 @@
       <c r="E629" s="7"/>
       <c r="F629" s="7"/>
       <c r="G629" s="7" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="H629" s="7"/>
       <c r="I629" s="7" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
     </row>
     <row r="630" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13184,10 +13216,10 @@
         <v>4</v>
       </c>
       <c r="B630" s="7" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="C630" s="7" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="D630" s="7" t="s">
         <v>24</v>
@@ -13199,7 +13231,7 @@
       <c r="G630" s="7"/>
       <c r="H630" s="7"/>
       <c r="I630" s="7" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
     </row>
     <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13210,29 +13242,29 @@
         <v>162</v>
       </c>
       <c r="C631" s="20" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D631" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E631" s="20" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F631" s="20" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="G631" s="20"/>
       <c r="H631" s="20"/>
       <c r="I631" s="20" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="633" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="1" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
     </row>
     <row r="635" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13269,24 +13301,24 @@
         <v>1</v>
       </c>
       <c r="B636" s="10" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C636" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D636" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E636" s="8" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="F636" s="8" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="G636" s="8"/>
       <c r="H636" s="8"/>
       <c r="I636" s="8" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="637" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13294,7 +13326,7 @@
         <v>2</v>
       </c>
       <c r="B637" s="7" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="C637" s="7" t="s">
         <v>81</v>
@@ -13305,11 +13337,11 @@
       <c r="E637" s="7"/>
       <c r="F637" s="7"/>
       <c r="G637" s="7" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="H637" s="7"/>
       <c r="I637" s="7" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
     </row>
     <row r="638" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13317,10 +13349,10 @@
         <v>3</v>
       </c>
       <c r="B638" s="7" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="C638" s="7" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="D638" s="7" t="s">
         <v>13</v>
@@ -13330,7 +13362,7 @@
       <c r="G638" s="7"/>
       <c r="H638" s="7"/>
       <c r="I638" s="7" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13341,29 +13373,29 @@
         <v>162</v>
       </c>
       <c r="C639" s="20" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D639" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E639" s="20" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F639" s="20" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="G639" s="20"/>
       <c r="H639" s="20"/>
       <c r="I639" s="20" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="1" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
     </row>
     <row r="643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13400,24 +13432,24 @@
         <v>1</v>
       </c>
       <c r="B644" s="10" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C644" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D644" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E644" s="8" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="F644" s="8" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="G644" s="8"/>
       <c r="H644" s="8"/>
       <c r="I644" s="8" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="645" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13425,7 +13457,7 @@
         <v>2</v>
       </c>
       <c r="B645" s="7" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="C645" s="7" t="s">
         <v>81</v>
@@ -13436,11 +13468,11 @@
       <c r="E645" s="7"/>
       <c r="F645" s="7"/>
       <c r="G645" s="7" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="H645" s="7"/>
       <c r="I645" s="7" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
     </row>
     <row r="646" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13448,7 +13480,7 @@
         <v>3</v>
       </c>
       <c r="B646" s="7" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="C646" s="7" t="s">
         <v>78</v>
@@ -13461,7 +13493,7 @@
       <c r="G646" s="7"/>
       <c r="H646" s="7"/>
       <c r="I646" s="7" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13472,29 +13504,29 @@
         <v>162</v>
       </c>
       <c r="C647" s="20" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D647" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E647" s="20" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F647" s="20" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="G647" s="20"/>
       <c r="H647" s="20"/>
       <c r="I647" s="20" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="649" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="1" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="B649" s="1" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
     </row>
     <row r="651" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13531,24 +13563,24 @@
         <v>1</v>
       </c>
       <c r="B652" s="10" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C652" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D652" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E652" s="8" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="F652" s="8" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="G652" s="8"/>
       <c r="H652" s="8"/>
       <c r="I652" s="8" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="653" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13556,7 +13588,7 @@
         <v>2</v>
       </c>
       <c r="B653" s="7" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="C653" s="7" t="s">
         <v>81</v>
@@ -13567,11 +13599,11 @@
       <c r="E653" s="7"/>
       <c r="F653" s="7"/>
       <c r="G653" s="7" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="H653" s="7"/>
       <c r="I653" s="7" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
     </row>
     <row r="654" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13579,10 +13611,10 @@
         <v>3</v>
       </c>
       <c r="B654" s="7" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
       <c r="C654" s="7" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="D654" s="7" t="s">
         <v>13</v>
@@ -13592,7 +13624,7 @@
       <c r="G654" s="7"/>
       <c r="H654" s="7"/>
       <c r="I654" s="7" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13600,7 +13632,7 @@
         <v>4</v>
       </c>
       <c r="B655" s="8" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="C655" s="8" t="s">
         <v>81</v>
@@ -13613,7 +13645,7 @@
       <c r="G655" s="8"/>
       <c r="H655" s="8"/>
       <c r="I655" s="8" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13624,29 +13656,29 @@
         <v>162</v>
       </c>
       <c r="C656" s="20" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D656" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E656" s="20" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F656" s="20" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="G656" s="20"/>
       <c r="H656" s="20"/>
       <c r="I656" s="20" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="658" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="1" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="B658" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="660" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13683,24 +13715,24 @@
         <v>1</v>
       </c>
       <c r="B661" s="10" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C661" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D661" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E661" s="8" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="F661" s="8" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="G661" s="8"/>
       <c r="H661" s="8"/>
       <c r="I661" s="8" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="662" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13708,7 +13740,7 @@
         <v>2</v>
       </c>
       <c r="B662" s="11" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C662" s="7" t="s">
         <v>40</v>
@@ -13727,7 +13759,7 @@
         <v>42</v>
       </c>
       <c r="I662" s="7" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
     </row>
     <row r="663" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13752,7 +13784,7 @@
         <v>414</v>
       </c>
       <c r="I663" s="8" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="664" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13760,7 +13792,7 @@
         <v>5</v>
       </c>
       <c r="B664" s="8" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C664" s="8" t="s">
         <v>366</v>
@@ -13773,7 +13805,7 @@
       <c r="G664" s="8"/>
       <c r="H664" s="8"/>
       <c r="I664" s="8" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
     </row>
     <row r="665" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13794,7 +13826,7 @@
       <c r="G665" s="7"/>
       <c r="H665" s="7"/>
       <c r="I665" s="7" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
     </row>
     <row r="666" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13802,10 +13834,10 @@
         <v>7</v>
       </c>
       <c r="B666" s="8" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="C666" s="8" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="D666" s="8" t="s">
         <v>24</v>
@@ -13815,7 +13847,7 @@
       <c r="G666" s="8"/>
       <c r="H666" s="8"/>
       <c r="I666" s="8" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13826,29 +13858,29 @@
         <v>162</v>
       </c>
       <c r="C667" s="20" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D667" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E667" s="20" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F667" s="20" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="G667" s="20"/>
       <c r="H667" s="20"/>
       <c r="I667" s="20" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="669" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="1" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
     </row>
     <row r="671" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13894,7 +13926,7 @@
         <v>13</v>
       </c>
       <c r="E672" s="8" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="F672" s="8" t="s">
         <v>450</v>
@@ -13902,7 +13934,7 @@
       <c r="G672" s="8"/>
       <c r="H672" s="8"/>
       <c r="I672" s="8" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
     </row>
     <row r="673" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13929,7 +13961,7 @@
         <v>42</v>
       </c>
       <c r="I673" s="7" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
     </row>
     <row r="674" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13940,7 +13972,7 @@
         <v>358</v>
       </c>
       <c r="C674" s="8" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="D674" s="8" t="s">
         <v>13</v>
@@ -13954,7 +13986,7 @@
         <v>414</v>
       </c>
       <c r="I674" s="8" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13962,24 +13994,24 @@
         <v>4</v>
       </c>
       <c r="B675" s="11" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C675" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D675" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E675" s="7" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F675" s="7" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="G675" s="7"/>
       <c r="H675" s="7"/>
       <c r="I675" s="7" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
     </row>
     <row r="676" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13987,7 +14019,7 @@
         <v>5</v>
       </c>
       <c r="B676" s="8" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C676" s="8" t="s">
         <v>366</v>
@@ -14000,7 +14032,7 @@
       <c r="G676" s="8"/>
       <c r="H676" s="8"/>
       <c r="I676" s="8" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
     </row>
     <row r="677" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14021,7 +14053,7 @@
       <c r="G677" s="7"/>
       <c r="H677" s="7"/>
       <c r="I677" s="7" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14029,7 +14061,7 @@
         <v>7</v>
       </c>
       <c r="B678" s="8" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="C678" s="8" t="s">
         <v>63</v>
@@ -14043,10 +14075,10 @@
         <v>194</v>
       </c>
       <c r="H678" s="8" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="I678" s="8" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14057,29 +14089,29 @@
         <v>162</v>
       </c>
       <c r="C679" s="20" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D679" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E679" s="20" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F679" s="20" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="G679" s="20"/>
       <c r="H679" s="20"/>
       <c r="I679" s="20" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="1" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="B681" s="1" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
     </row>
     <row r="683" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14087,16 +14119,16 @@
         <v>2</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="C683" s="2" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="D683" s="2" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="E683" s="2" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="F683" s="2" t="s">
         <v>7</v>
@@ -14105,7 +14137,7 @@
         <v>8</v>
       </c>
       <c r="H683" s="2" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="I683" s="2" t="s">
         <v>10</v>
@@ -14116,7 +14148,7 @@
         <v>1</v>
       </c>
       <c r="B684" s="10" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="C684" s="8" t="s">
         <v>484</v>
@@ -14125,7 +14157,7 @@
         <v>13</v>
       </c>
       <c r="E684" s="8" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="F684" s="8" t="s">
         <v>522</v>
@@ -14133,7 +14165,7 @@
       <c r="G684" s="8"/>
       <c r="H684" s="8"/>
       <c r="I684" s="8" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
     </row>
     <row r="685" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14160,7 +14192,7 @@
         <v>42</v>
       </c>
       <c r="I685" s="7" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
     </row>
     <row r="686" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14171,7 +14203,7 @@
         <v>358</v>
       </c>
       <c r="C686" s="8" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="D686" s="8" t="s">
         <v>13</v>
@@ -14185,7 +14217,7 @@
         <v>414</v>
       </c>
       <c r="I686" s="8" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
     </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14193,24 +14225,24 @@
         <v>4</v>
       </c>
       <c r="B687" s="11" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C687" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D687" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E687" s="7" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F687" s="7" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="G687" s="7"/>
       <c r="H687" s="7"/>
       <c r="I687" s="7" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
     </row>
     <row r="688" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14218,7 +14250,7 @@
         <v>5</v>
       </c>
       <c r="B688" s="8" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C688" s="8" t="s">
         <v>366</v>
@@ -14231,7 +14263,7 @@
       <c r="G688" s="8"/>
       <c r="H688" s="8"/>
       <c r="I688" s="8" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
     </row>
     <row r="689" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14252,7 +14284,7 @@
       <c r="G689" s="7"/>
       <c r="H689" s="7"/>
       <c r="I689" s="7" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
     </row>
     <row r="690" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14260,7 +14292,7 @@
         <v>7</v>
       </c>
       <c r="B690" s="8" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="C690" s="8" t="s">
         <v>63</v>
@@ -14274,10 +14306,10 @@
         <v>194</v>
       </c>
       <c r="H690" s="8" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="I690" s="8" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
     </row>
     <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14288,29 +14320,29 @@
         <v>162</v>
       </c>
       <c r="C691" s="20" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D691" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E691" s="20" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F691" s="20" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="G691" s="20"/>
       <c r="H691" s="20"/>
       <c r="I691" s="20" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="693" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="1" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="B693" s="1" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
     </row>
     <row r="695" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14318,16 +14350,16 @@
         <v>2</v>
       </c>
       <c r="B695" s="2" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="C695" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D695" s="2" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="E695" s="2" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="F695" s="2" t="s">
         <v>7</v>
@@ -14336,7 +14368,7 @@
         <v>8</v>
       </c>
       <c r="H695" s="2" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="I695" s="2" t="s">
         <v>10</v>
@@ -14356,15 +14388,15 @@
         <v>13</v>
       </c>
       <c r="E696" s="8" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="F696" s="8" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="G696" s="8"/>
       <c r="H696" s="8"/>
       <c r="I696" s="8" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
     </row>
     <row r="697" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14391,7 +14423,7 @@
         <v>42</v>
       </c>
       <c r="I697" s="7" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
     </row>
     <row r="698" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14402,7 +14434,7 @@
         <v>358</v>
       </c>
       <c r="C698" s="8" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="D698" s="8" t="s">
         <v>13</v>
@@ -14416,7 +14448,7 @@
         <v>414</v>
       </c>
       <c r="I698" s="8" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
     </row>
     <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14424,24 +14456,24 @@
         <v>4</v>
       </c>
       <c r="B699" s="11" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C699" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D699" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E699" s="7" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F699" s="7" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="G699" s="7"/>
       <c r="H699" s="7"/>
       <c r="I699" s="7" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
     </row>
     <row r="700" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14449,7 +14481,7 @@
         <v>5</v>
       </c>
       <c r="B700" s="8" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C700" s="8" t="s">
         <v>366</v>
@@ -14462,7 +14494,7 @@
       <c r="G700" s="8"/>
       <c r="H700" s="8"/>
       <c r="I700" s="8" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
     </row>
     <row r="701" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14473,7 +14505,7 @@
         <v>378</v>
       </c>
       <c r="C701" s="7" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="D701" s="7" t="s">
         <v>13</v>
@@ -14483,7 +14515,7 @@
       <c r="G701" s="7"/>
       <c r="H701" s="7"/>
       <c r="I701" s="7" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
     </row>
     <row r="702" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14491,7 +14523,7 @@
         <v>7</v>
       </c>
       <c r="B702" s="8" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="C702" s="8" t="s">
         <v>63</v>
@@ -14505,10 +14537,10 @@
         <v>194</v>
       </c>
       <c r="H702" s="8" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="I702" s="8" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
     </row>
     <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14519,29 +14551,29 @@
         <v>162</v>
       </c>
       <c r="C703" s="20" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="D703" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E703" s="20" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F703" s="20" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="G703" s="20"/>
       <c r="H703" s="20"/>
       <c r="I703" s="20" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="705" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A705" s="1" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="B705" s="22" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
     </row>
     <row r="707" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14549,16 +14581,16 @@
         <v>2</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="C707" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D707" s="2" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="E707" s="2" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="F707" s="2" t="s">
         <v>7</v>
@@ -14567,7 +14599,7 @@
         <v>8</v>
       </c>
       <c r="H707" s="2" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="I707" s="2" t="s">
         <v>10</v>
@@ -14578,7 +14610,7 @@
         <v>1</v>
       </c>
       <c r="B708" s="10" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="C708" s="8" t="s">
         <v>109</v>
@@ -14595,7 +14627,7 @@
       </c>
       <c r="H708" s="8"/>
       <c r="I708" s="8" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
     </row>
     <row r="709" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14616,7 +14648,7 @@
       <c r="G709" s="7"/>
       <c r="H709" s="7"/>
       <c r="I709" s="7" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
     </row>
     <row r="710" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14624,7 +14656,7 @@
         <v>3</v>
       </c>
       <c r="B710" s="8" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="C710" s="8" t="s">
         <v>265</v>
@@ -14637,7 +14669,7 @@
       <c r="G710" s="8"/>
       <c r="H710" s="8"/>
       <c r="I710" s="8" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
     </row>
     <row r="711" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14645,7 +14677,7 @@
         <v>4</v>
       </c>
       <c r="B711" s="7" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="C711" s="7" t="s">
         <v>265</v>
@@ -14658,7 +14690,7 @@
       <c r="G711" s="7"/>
       <c r="H711" s="7"/>
       <c r="I711" s="7" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
     </row>
     <row r="712" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14666,10 +14698,10 @@
         <v>5</v>
       </c>
       <c r="B712" s="8" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c r="C712" s="8" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="D712" s="8" t="s">
         <v>24</v>
@@ -14679,7 +14711,7 @@
       <c r="G712" s="8"/>
       <c r="H712" s="8"/>
       <c r="I712" s="8" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
     </row>
     <row r="713" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14687,10 +14719,10 @@
         <v>6</v>
       </c>
       <c r="B713" s="7" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="C713" s="7" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="D713" s="7" t="s">
         <v>13</v>
@@ -14700,7 +14732,7 @@
       <c r="G713" s="7"/>
       <c r="H713" s="7"/>
       <c r="I713" s="7" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
     </row>
     <row r="714" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14708,7 +14740,7 @@
         <v>7</v>
       </c>
       <c r="B714" s="8" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c r="C714" s="8" t="s">
         <v>63</v>
@@ -14719,13 +14751,13 @@
       <c r="E714" s="8"/>
       <c r="F714" s="8"/>
       <c r="G714" s="8" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="H714" s="8" t="s">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="I714" s="8" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
     </row>
     <row r="715" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14733,7 +14765,7 @@
         <v>8</v>
       </c>
       <c r="B715" s="7" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="C715" s="7" t="s">
         <v>63</v>
@@ -14744,13 +14776,13 @@
       <c r="E715" s="7"/>
       <c r="F715" s="7"/>
       <c r="G715" s="7" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="H715" s="7" t="s">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="I715" s="7" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
     </row>
     <row r="716" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14763,10 +14795,10 @@
     </row>
     <row r="717" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A717" s="1" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
       <c r="B717" s="22" t="s">
-        <v>826</v>
+        <v>829</v>
       </c>
     </row>
     <row r="719" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14774,16 +14806,16 @@
         <v>2</v>
       </c>
       <c r="B719" s="2" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="C719" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D719" s="2" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="E719" s="2" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="F719" s="2" t="s">
         <v>7</v>
@@ -14792,7 +14824,7 @@
         <v>8</v>
       </c>
       <c r="H719" s="2" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="I719" s="2" t="s">
         <v>10</v>
@@ -14803,7 +14835,7 @@
         <v>1</v>
       </c>
       <c r="B720" s="10" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
       <c r="C720" s="8" t="s">
         <v>109</v>
@@ -14815,12 +14847,12 @@
         <v>649</v>
       </c>
       <c r="F720" s="8" t="s">
-        <v>827</v>
+        <v>830</v>
       </c>
       <c r="G720" s="8"/>
       <c r="H720" s="8"/>
       <c r="I720" s="8" t="s">
-        <v>828</v>
+        <v>831</v>
       </c>
     </row>
     <row r="721" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14828,10 +14860,10 @@
         <v>2</v>
       </c>
       <c r="B721" s="11" t="s">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c r="C721" s="7" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="D721" s="7" t="s">
         <v>13</v>
@@ -14843,15 +14875,15 @@
       <c r="G721" s="7"/>
       <c r="H721" s="7"/>
       <c r="I721" s="7" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
     </row>
     <row r="724" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A724" s="1" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
       <c r="B724" s="1" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
     </row>
     <row r="726" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14905,7 +14937,7 @@
       <c r="G727" s="8"/>
       <c r="H727" s="8"/>
       <c r="I727" s="8" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
     </row>
     <row r="728" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14930,15 +14962,15 @@
       <c r="G728" s="7"/>
       <c r="H728" s="7"/>
       <c r="I728" s="7" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
     </row>
     <row r="731" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A731" s="1" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="B731" s="1" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
     </row>
     <row r="733" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14975,7 +15007,7 @@
         <v>1</v>
       </c>
       <c r="B734" s="10" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="C734" s="8" t="s">
         <v>390</v>
@@ -14992,7 +15024,7 @@
       <c r="G734" s="8"/>
       <c r="H734" s="8"/>
       <c r="I734" s="8" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
     </row>
     <row r="735" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15000,7 +15032,7 @@
         <v>2</v>
       </c>
       <c r="B735" s="7" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="C735" s="7" t="s">
         <v>84</v>
@@ -15019,7 +15051,7 @@
       </c>
       <c r="H735" s="7"/>
       <c r="I735" s="7" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
     </row>
     <row r="736" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15027,7 +15059,7 @@
         <v>3</v>
       </c>
       <c r="B736" s="8" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="C736" s="8" t="s">
         <v>84</v>
@@ -15044,7 +15076,7 @@
       <c r="G736" s="8"/>
       <c r="H736" s="8"/>
       <c r="I736" s="8" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
     </row>
     <row r="737" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15052,7 +15084,7 @@
         <v>4</v>
       </c>
       <c r="B737" s="7" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="C737" s="7" t="s">
         <v>63</v>
@@ -15063,11 +15095,11 @@
       <c r="E737" s="7"/>
       <c r="F737" s="7"/>
       <c r="G737" s="7" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="H737" s="7"/>
       <c r="I737" s="7" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
     </row>
     <row r="738" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15075,7 +15107,7 @@
         <v>5</v>
       </c>
       <c r="B738" s="8" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="C738" s="8" t="s">
         <v>390</v>
@@ -15088,7 +15120,7 @@
       <c r="G738" s="8"/>
       <c r="H738" s="8"/>
       <c r="I738" s="8" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
     </row>
     <row r="739" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15096,7 +15128,7 @@
         <v>6</v>
       </c>
       <c r="B739" s="7" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="C739" s="7" t="s">
         <v>63</v>
@@ -15111,15 +15143,15 @@
       </c>
       <c r="H739" s="7"/>
       <c r="I739" s="7" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
     </row>
     <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A741" s="1" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="B741" s="1" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
     </row>
     <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15156,7 +15188,7 @@
         <v>1</v>
       </c>
       <c r="B744" s="10" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="C744" s="8" t="s">
         <v>294</v>
@@ -15165,15 +15197,15 @@
         <v>13</v>
       </c>
       <c r="E744" s="8" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F744" s="8" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="G744" s="8"/>
       <c r="H744" s="8"/>
       <c r="I744" s="8" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
     </row>
     <row r="745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15190,10 +15222,10 @@
         <v>13</v>
       </c>
       <c r="E745" s="7" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F745" s="7" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="G745" s="7" t="s">
         <v>193</v>
@@ -15208,7 +15240,7 @@
         <v>3</v>
       </c>
       <c r="B746" s="8" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="C746" s="8" t="s">
         <v>366</v>
@@ -15221,7 +15253,7 @@
       <c r="G746" s="8"/>
       <c r="H746" s="8"/>
       <c r="I746" s="8" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
database is updated due to BranchMilkLog
</commit_message>
<xml_diff>
--- a/Data Dictionary Version 0.xlsx
+++ b/Data Dictionary Version 0.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="861">
   <si>
     <t xml:space="preserve">T2</t>
   </si>
@@ -1839,90 +1839,93 @@
     <t xml:space="preserve">BranchID</t>
   </si>
   <si>
+    <t xml:space="preserve">store local dairy id which is branch of current dairy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store date of which milk is given by local branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store date and time when milk data is entered in system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets 1 for morning and 0 for evening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMQuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store total milk quantity in that no of cylinder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TClyQuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store total cylinder quantity of that cylinder no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">char(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store cylinder no of cylinder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;=20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store fat of milk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store snf of milk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store water percentage in milk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto calculated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from {'0','1'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 for quantity in kg and 0 for litre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ArriveTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrival time of cylinder at dairy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport(TransID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transport id of driver who brings the cylinders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store milk type id no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FK, PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BranchPayLog</t>
+  </si>
+  <si>
     <t xml:space="preserve">MDBranch(BranchID)</t>
   </si>
   <si>
-    <t xml:space="preserve">store local dairy id which is branch of current dairy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Store date of which milk is given by local branch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store date and time when milk data is entered in system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sets 1 for morning and 0 for evening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TMQuantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store total milk quantity in that no of cylinder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TClyQuantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store total cylinder quantity of that cylinder no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">char(7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store cylinder no of cylinder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;=20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store fat of milk </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store snf of milk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store water percentage in milk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">auto calculated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from {'0','1'}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 for quantity in kg and 0 for litre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ArriveTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arrival time of cylinder at dairy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport(TransID)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transport id of driver who brings the cylinders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store milk type id no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BranchPayLog</t>
-  </si>
-  <si>
     <t xml:space="preserve">store date to which payment is being done</t>
   </si>
   <si>
@@ -1963,9 +1966,6 @@
   </si>
   <si>
     <t xml:space="preserve">store mobile no of the additional customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FK, PK</t>
   </si>
   <si>
     <t xml:space="preserve">T51</t>
@@ -2974,20 +2974,20 @@
   </sheetPr>
   <dimension ref="A3:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A529" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F542" activeCellId="0" sqref="F542"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A488" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C510" activeCellId="0" sqref="C510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -10828,12 +10828,12 @@
         <v>90</v>
       </c>
       <c r="F496" s="8" t="s">
-        <v>605</v>
+        <v>183</v>
       </c>
       <c r="G496" s="8"/>
       <c r="H496" s="8"/>
       <c r="I496" s="8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10860,7 +10860,7 @@
         <v>42</v>
       </c>
       <c r="I497" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10885,14 +10885,14 @@
         <v>414</v>
       </c>
       <c r="I498" s="8" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B499" s="7" t="s">
+      <c r="B499" s="11" t="s">
         <v>362</v>
       </c>
       <c r="C499" s="7" t="s">
@@ -10901,14 +10901,16 @@
       <c r="D499" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E499" s="7"/>
+      <c r="E499" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F499" s="7"/>
       <c r="G499" s="7" t="s">
         <v>194</v>
       </c>
       <c r="H499" s="7"/>
       <c r="I499" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10916,7 +10918,7 @@
         <v>5</v>
       </c>
       <c r="B500" s="8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C500" s="8" t="s">
         <v>366</v>
@@ -10929,7 +10931,7 @@
       <c r="G500" s="8"/>
       <c r="H500" s="8"/>
       <c r="I500" s="8" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10937,7 +10939,7 @@
         <v>6</v>
       </c>
       <c r="B501" s="7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C501" s="7" t="s">
         <v>109</v>
@@ -10950,7 +10952,7 @@
       <c r="G501" s="7"/>
       <c r="H501" s="7"/>
       <c r="I501" s="7" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10958,10 +10960,10 @@
         <v>7</v>
       </c>
       <c r="B502" s="8" t="s">
+        <v>613</v>
+      </c>
+      <c r="C502" s="8" t="s">
         <v>614</v>
-      </c>
-      <c r="C502" s="8" t="s">
-        <v>615</v>
       </c>
       <c r="D502" s="8" t="s">
         <v>13</v>
@@ -10971,7 +10973,7 @@
       <c r="G502" s="8"/>
       <c r="H502" s="8"/>
       <c r="I502" s="8" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10990,11 +10992,11 @@
       <c r="E503" s="7"/>
       <c r="F503" s="7"/>
       <c r="G503" s="7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="H503" s="7"/>
       <c r="I503" s="7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11013,11 +11015,11 @@
       <c r="E504" s="8"/>
       <c r="F504" s="8"/>
       <c r="G504" s="8" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="H504" s="8"/>
       <c r="I504" s="8" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11028,13 +11030,13 @@
         <v>371</v>
       </c>
       <c r="C505" s="14" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D505" s="14" t="s">
         <v>24</v>
       </c>
       <c r="I505" s="14" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11053,7 +11055,7 @@
       <c r="E506" s="8"/>
       <c r="F506" s="8"/>
       <c r="G506" s="8" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H506" s="8"/>
       <c r="I506" s="8" t="s">
@@ -11076,11 +11078,11 @@
       <c r="E507" s="5"/>
       <c r="F507" s="5"/>
       <c r="G507" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H507" s="5"/>
       <c r="I507" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11088,10 +11090,10 @@
         <v>13</v>
       </c>
       <c r="B508" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="C508" s="8" t="s">
         <v>625</v>
-      </c>
-      <c r="C508" s="8" t="s">
-        <v>626</v>
       </c>
       <c r="D508" s="8" t="s">
         <v>24</v>
@@ -11101,7 +11103,7 @@
       <c r="G508" s="8"/>
       <c r="H508" s="8"/>
       <c r="I508" s="8" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11112,7 +11114,7 @@
         <v>585</v>
       </c>
       <c r="C509" s="5" t="s">
-        <v>347</v>
+        <v>109</v>
       </c>
       <c r="D509" s="5" t="s">
         <v>13</v>
@@ -11121,12 +11123,12 @@
         <v>57</v>
       </c>
       <c r="F509" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G509" s="5"/>
       <c r="H509" s="5"/>
       <c r="I509" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11137,7 +11139,7 @@
         <v>346</v>
       </c>
       <c r="C510" s="8" t="s">
-        <v>347</v>
+        <v>109</v>
       </c>
       <c r="D510" s="8" t="s">
         <v>13</v>
@@ -11151,14 +11153,14 @@
       <c r="G510" s="8"/>
       <c r="H510" s="8"/>
       <c r="I510" s="8" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="511" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="B511" s="5" t="s">
+      <c r="B511" s="17" t="s">
         <v>162</v>
       </c>
       <c r="C511" s="5" t="s">
@@ -11168,7 +11170,7 @@
         <v>13</v>
       </c>
       <c r="E511" s="5" t="s">
-        <v>57</v>
+        <v>630</v>
       </c>
       <c r="F511" s="5" t="s">
         <v>254</v>
@@ -11233,12 +11235,12 @@
         <v>90</v>
       </c>
       <c r="F516" s="8" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
       <c r="G516" s="8"/>
       <c r="H516" s="8"/>
       <c r="I516" s="8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11265,7 +11267,7 @@
         <v>42</v>
       </c>
       <c r="I517" s="7" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11290,7 +11292,7 @@
         <v>414</v>
       </c>
       <c r="I518" s="8" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11311,7 +11313,7 @@
       <c r="G519" s="7"/>
       <c r="H519" s="7"/>
       <c r="I519" s="7" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11332,7 +11334,7 @@
       <c r="G520" s="8"/>
       <c r="H520" s="8"/>
       <c r="I520" s="8" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11353,7 +11355,7 @@
       <c r="G521" s="5"/>
       <c r="H521" s="5"/>
       <c r="I521" s="5" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11374,7 +11376,7 @@
       <c r="G522" s="8"/>
       <c r="H522" s="8"/>
       <c r="I522" s="8" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11422,7 +11424,7 @@
       </c>
       <c r="H524" s="8"/>
       <c r="I524" s="8" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11498,10 +11500,10 @@
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="9" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B530" s="9" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11538,7 +11540,7 @@
         <v>1</v>
       </c>
       <c r="B533" s="7" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C533" s="7" t="s">
         <v>71</v>
@@ -11549,11 +11551,11 @@
       <c r="E533" s="7"/>
       <c r="F533" s="7"/>
       <c r="G533" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="H533" s="7"/>
       <c r="I533" s="7" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11577,10 +11579,10 @@
         <v>511</v>
       </c>
       <c r="H534" s="7" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="I534" s="7" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11597,7 +11599,7 @@
         <v>13</v>
       </c>
       <c r="E535" s="8" t="s">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="F535" s="8" t="s">
         <v>254</v>
@@ -11744,7 +11746,7 @@
       </c>
       <c r="H545" s="7"/>
       <c r="I545" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11761,7 +11763,7 @@
         <v>13</v>
       </c>
       <c r="E546" s="8" t="s">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="F546" s="8" t="s">
         <v>254</v>
@@ -11853,7 +11855,7 @@
       <c r="E550" s="7"/>
       <c r="F550" s="7"/>
       <c r="G550" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="H550" s="7"/>
       <c r="I550" s="7" t="s">
@@ -12014,7 +12016,7 @@
         <v>57</v>
       </c>
       <c r="F559" s="8" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G559" s="8"/>
       <c r="H559" s="8"/>
@@ -12069,7 +12071,7 @@
         <v>8</v>
       </c>
       <c r="B562" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C562" s="7" t="s">
         <v>677</v>
@@ -12082,7 +12084,7 @@
       <c r="G562" s="7"/>
       <c r="H562" s="7"/>
       <c r="I562" s="7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12101,7 +12103,7 @@
       <c r="E563" s="8"/>
       <c r="F563" s="8"/>
       <c r="G563" s="8" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="H563" s="8"/>
       <c r="I563" s="8" t="s">
@@ -12124,11 +12126,11 @@
       <c r="E564" s="7"/>
       <c r="F564" s="7"/>
       <c r="G564" s="7" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="H564" s="7"/>
       <c r="I564" s="7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12332,7 +12334,7 @@
         <v>42</v>
       </c>
       <c r="I576" s="7" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="577" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14821,7 +14823,7 @@
         <v>13</v>
       </c>
       <c r="E719" s="8" t="s">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="F719" s="8" t="s">
         <v>830</v>
@@ -15116,7 +15118,7 @@
       <c r="E738" s="7"/>
       <c r="F738" s="7"/>
       <c r="G738" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H738" s="7"/>
       <c r="I738" s="7" t="s">

</xml_diff>

<commit_message>
Updation in database table on 30 Jan 2019
</commit_message>
<xml_diff>
--- a/Data Dictionary Version 0.xlsx
+++ b/Data Dictionary Version 0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2980" uniqueCount="878">
   <si>
     <t xml:space="preserve">T2</t>
   </si>
@@ -2655,6 +2655,57 @@
   </si>
   <si>
     <t xml:space="preserve">store gst percent on product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HighOfDairy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store dairy id no of local diary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store highest producer id no of local dairy for next customer registeration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store highest of consumer id no of dairy for next registration of consumer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserPass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store customer id for saving user name and password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Char (40)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[A-Za-z0-9\s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store user name for dairy customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userPass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[A-Za-z0-9\s\\special_characters]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must be greater than 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store user password for dairy customer</t>
   </si>
 </sst>
 </file>
@@ -2754,7 +2805,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -2774,6 +2825,13 @@
       <right style="thin"/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -2802,7 +2860,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2895,6 +2953,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2972,23 +3034,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:I65536"/>
+  <dimension ref="A3:I1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A488" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C510" activeCellId="0" sqref="C510"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A738" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C753" activeCellId="0" sqref="C753"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15233,6 +15295,229 @@
       <c r="H745" s="8"/>
       <c r="I745" s="8" t="s">
         <v>860</v>
+      </c>
+    </row>
+    <row r="747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A747" s="23" t="s">
+        <v>861</v>
+      </c>
+      <c r="B747" s="23" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A749" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B749" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C749" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D749" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E749" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F749" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G749" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H749" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I749" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A750" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B750" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C750" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D750" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E750" s="8" t="s">
+        <v>731</v>
+      </c>
+      <c r="F750" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G750" s="8"/>
+      <c r="H750" s="8"/>
+      <c r="I750" s="8" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A751" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B751" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C751" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D751" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E751" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F751" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G751" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="H751" s="7"/>
+      <c r="I751" s="7" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A752" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B752" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C752" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D752" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E752" s="8"/>
+      <c r="F752" s="8"/>
+      <c r="G752" s="8"/>
+      <c r="H752" s="8"/>
+      <c r="I752" s="8" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="755" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A755" s="23" t="s">
+        <v>866</v>
+      </c>
+      <c r="B755" s="23" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="756" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A757" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B757" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C757" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D757" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E757" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F757" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G757" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H757" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I757" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="758" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A758" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B758" s="10" t="s">
+        <v>868</v>
+      </c>
+      <c r="C758" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D758" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E758" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="F758" s="8"/>
+      <c r="G758" s="8"/>
+      <c r="H758" s="8"/>
+      <c r="I758" s="8" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="759" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A759" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B759" s="7" t="s">
+        <v>870</v>
+      </c>
+      <c r="C759" s="7" t="s">
+        <v>871</v>
+      </c>
+      <c r="D759" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E759" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F759" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G759" s="7" t="s">
+        <v>872</v>
+      </c>
+      <c r="H759" s="7"/>
+      <c r="I759" s="7" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A760" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B760" s="8" t="s">
+        <v>874</v>
+      </c>
+      <c r="C760" s="8" t="s">
+        <v>871</v>
+      </c>
+      <c r="D760" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E760" s="8"/>
+      <c r="F760" s="8"/>
+      <c r="G760" s="8" t="s">
+        <v>875</v>
+      </c>
+      <c r="H760" s="8" t="s">
+        <v>876</v>
+      </c>
+      <c r="I760" s="8" t="s">
+        <v>877</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15249,7 +15534,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -15264,18 +15549,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -15290,18 +15575,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>